<commit_message>
Added Submit State Report
</commit_message>
<xml_diff>
--- a/testdata/TrackerDataChrome.xlsx
+++ b/testdata/TrackerDataChrome.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5BF28-3ABE-40D7-8CF3-06E1727D0DDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A9334-3328-43BD-82EC-5291A935035B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holder" sheetId="2" r:id="rId1"/>
     <sheet name="Letter" sheetId="3" r:id="rId2"/>
     <sheet name="RyanMail" sheetId="4" r:id="rId3"/>
     <sheet name="Report" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="219">
   <si>
     <t>P</t>
   </si>
@@ -622,9 +624,6 @@
     <t>SD</t>
   </si>
   <si>
-    <t>TS</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -647,6 +646,48 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>ReportCategory</t>
+  </si>
+  <si>
+    <t>HolderList</t>
+  </si>
+  <si>
+    <t>ReportGroup</t>
+  </si>
+  <si>
+    <t>ReportDetail</t>
+  </si>
+  <si>
+    <t>ReportType</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Separate</t>
+  </si>
+  <si>
+    <t>Finalize</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>HolderList2</t>
+  </si>
+  <si>
+    <t>States2</t>
   </si>
 </sst>
 </file>
@@ -697,13 +738,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1536,7 +1580,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:E21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2160,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A153BF37-F317-4CB7-B885-8B1692BAAF90}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2533,7 +2577,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>3</v>
@@ -2541,7 +2585,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>3</v>
@@ -2557,7 +2601,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>3</v>
@@ -2565,7 +2609,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>3</v>
@@ -2573,7 +2617,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>3</v>
@@ -2581,7 +2625,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>3</v>
@@ -2589,7 +2633,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>3</v>
@@ -2597,7 +2641,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>3</v>
@@ -2605,7 +2649,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>3</v>
@@ -2615,4 +2659,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B07ACD-967D-4D9A-8A25-9E631168A653}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6914831-CE84-448A-BA5C-2EE1386E189D}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>